<commit_message>
Package excel and SQL Query updated - BASHA
</commit_message>
<xml_diff>
--- a/Documentation/PackageDetails.xlsx
+++ b/Documentation/PackageDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215"/>
+    <workbookView windowWidth="28800" windowHeight="12228"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Package ID</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Text 3</t>
   </si>
   <si>
+    <t>Visible In Grid</t>
+  </si>
+  <si>
     <t>100</t>
   </si>
   <si>
@@ -64,6 +67,9 @@
     <t>K2 regulations</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>5 Annual Reports</t>
   </si>
   <si>
@@ -104,6 +110,18 @@
   </si>
   <si>
     <t>UNLIMITED</t>
+  </si>
+  <si>
+    <t>Extra User</t>
+  </si>
+  <si>
+    <t>Until Accounting Company Package Period</t>
+  </si>
+  <si>
+    <t>ADD-ON</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -111,10 +129,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -130,6 +148,29 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -141,56 +182,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -204,6 +208,37 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -211,22 +246,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,39 +281,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,43 +304,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,79 +448,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,55 +472,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,21 +509,6 @@
       </top>
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,6 +537,45 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -552,8 +594,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -568,175 +610,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -761,52 +779,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1104,13 +1122,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="$A8:$XFD1048576"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="18.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="18.7777777777778" customWidth="1"/>
@@ -1121,9 +1139,10 @@
     <col min="7" max="7" width="18.7777777777778" customWidth="1"/>
     <col min="8" max="8" width="24.5555555555556" customWidth="1"/>
     <col min="9" max="9" width="20.8888888888889" customWidth="1"/>
+    <col min="10" max="10" width="17.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.15" spans="1:9">
+    <row r="1" ht="15.15" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1151,173 +1170,224 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" ht="15.15" spans="1:9">
+    <row r="2" ht="15.15" spans="1:10">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3">
         <v>399</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" ht="15.15" spans="1:9">
+    <row r="3" ht="15.15" spans="1:10">
       <c r="A3" s="6">
         <v>200</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="6">
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="6">
         <v>1499</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="4" ht="15.15" spans="1:9">
+    <row r="4" ht="15.15" spans="1:10">
       <c r="A4" s="6">
         <v>300</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="6">
         <v>10</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="6">
         <v>2499</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="5" ht="15.15" spans="1:9">
+    <row r="5" ht="15.15" spans="1:10">
       <c r="A5" s="6">
         <v>400</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6">
         <v>50</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" s="6">
         <v>2499</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="6" ht="15.15" spans="1:9">
+    <row r="6" ht="15.15" spans="1:10">
       <c r="A6" s="6">
         <v>500</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6" s="6">
         <v>100</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E6" s="6">
         <v>999</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" ht="15.15" spans="1:10">
       <c r="A7" s="6">
         <v>600</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" s="6">
         <v>9999999</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E7" s="6">
         <v>4999</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" ht="15.15" spans="1:10">
+      <c r="A8" s="6">
+        <v>700</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6">
+        <v>300</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>